<commit_message>
Added bg pix to itemlist.  switched to siteData json.  componentized itemlist.
</commit_message>
<xml_diff>
--- a/public/cges/content.xlsx
+++ b/public/cges/content.xlsx
@@ -5,23 +5,25 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="FAQ" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="CardTypes" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Card Types" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Main Categories" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Projects Categories" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Carousel" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Landing" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="About" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Women on Death Row" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Women on Death Row Categories" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Fellows Cards" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Toolkit Cards" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="News &amp; Events Cards" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Resource Hub Cards" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="Women on Death Row Cards" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Landing Image Example" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Landing Parallax Example" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="About" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Women on Death Row" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Women on Death Row Categories" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Fellows Cards" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Toolkit Cards" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="News &amp; Events Cards" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Resource Hub Cards" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="Women on Death Row Cards" sheetId="16" state="visible" r:id="rId17"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="217">
   <si>
     <t xml:space="preserve">Organization:</t>
   </si>
@@ -279,43 +281,46 @@
     <t xml:space="preserve">Type</t>
   </si>
   <si>
-    <t xml:space="preserve">FgColor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BgColor</t>
+    <t xml:space="preserve">Foreground</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
   </si>
   <si>
     <t xml:space="preserve">space</t>
   </si>
   <si>
-    <t xml:space="preserve">#E6A0C4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Center on Gender and Extreme Sentencing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Our vision and purpose is to strive to create a world where extreme sentencing is replaced with justice practices centered on restoration and healing instead of retribution and punishment.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">normal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Mission of the Center on Gender and Extreme Sentencing (CGES) is to expose intersectional discrimination practices within the criminal legal system.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#C6CDF7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We seek to combat extreme sentencing by revealing the contradictions, injustices, and biases of these punishments specifically when used against marginalized populations including women, people of color, transgender individuals, poor people, trauma and abuse survivors, and those with disabilities.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Problem: The issue of gender discrimination in sentencing is deeply urgent and profoundly misunderstood.</t>
-  </si>
-  <si>
     <t xml:space="preserve">white</t>
   </si>
   <si>
-    <t xml:space="preserve">Although women are the fastest growing population of incarcerated people, perceptions that they receive preferential treatment from the criminal legal system abound.</t>
+    <t xml:space="preserve">Landing Image Example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bg-image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">landingimg.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content contained in landing image example sheet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Landing Parallax Example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bg-parallax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">landingplx.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content contained in landing parallax example sheet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#D8A499</t>
   </si>
   <si>
     <r>
@@ -344,6 +349,7 @@
         <color rgb="FF000000"/>
         <rFont val="padmaa-Bold.1.1"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"</t>
     </r>
@@ -352,7 +358,7 @@
     <t xml:space="preserve">In reality, women have suffered the most in the era of mass incarceration, with female incarceration increasing by 700% since 1980, more than double the rate of male incarceration for the same period.</t>
   </si>
   <si>
-    <t xml:space="preserve">#D8A499</t>
+    <t xml:space="preserve">normal</t>
   </si>
   <si>
     <t xml:space="preserve">1/39 compared to 1/59</t>
@@ -365,6 +371,36 @@
   </si>
   <si>
     <t xml:space="preserve">The result is a prison system filled with the most vulnerable members of society, whose identities sit at the intersection of multiple forms of marginalization. Most have been victims long before they entered the system as perpetrators, yet were denied assistance and intervention when they needed it most. We believe in uplifting these individuals, because we understand that their lived experiences have the power to shed light on the cruelties and injustices of the criminal legal system. Their stories hold the key to transforming the system by moving it away from retribution and punishment and toward rehabilitation and healing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transparent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center on Gender and Extreme Sentencing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#E6A0C4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our vision and purpose is to strive to create a world where extreme sentencing is replaced with justice practices centered on restoration and healing instead of retribution and punishment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The issue of gender discrimination in sentencing is deeply urgent and profoundly misunderstood.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Although women are the fastest growing population of incarcerated people, perceptions that they receive preferential treatment from the criminal legal system abound.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#C6CDF7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The CGES Mission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We seek expose intersectional discrimination practices within the criminal legal system and combat extreme sentencing by revealing the contradictions, injustices, and biases of these punishments specifically when used against marginalized populations including women, people of color, transgender individuals, poor people, trauma and abuse survivors, and those with disabilities.</t>
   </si>
   <si>
     <t xml:space="preserve">Our Team</t>
@@ -690,7 +726,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -721,29 +757,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="padmaa-Bold.1.1"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="padmaa-Bold.1.1"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -795,7 +813,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -812,35 +830,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -867,7 +869,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -915,61 +917,34 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="I33" activeCellId="0" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -988,153 +963,50 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E2" s="1" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="1" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1153,35 +1025,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -1192,45 +1064,22 @@
         <v>134</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1249,35 +1098,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -1285,71 +1134,117 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>138</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1368,13 +1263,228 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.18"/>
   </cols>
@@ -1384,22 +1494,22 @@
         <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -1407,88 +1517,88 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>141</v>
+      <c r="A3" s="5" t="s">
+        <v>152</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="H3" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>143</v>
+      <c r="A4" s="5" t="s">
+        <v>154</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="H4" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>144</v>
+      <c r="A5" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="H5" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>145</v>
+      <c r="A6" s="5" t="s">
+        <v>156</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="H6" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
-        <v>146</v>
+      <c r="A7" s="5" t="s">
+        <v>157</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="H7" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
-        <v>147</v>
+      <c r="A8" s="5" t="s">
+        <v>158</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>42</v>
@@ -1496,65 +1606,65 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H9" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H10" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H11" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H12" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H13" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>42</v>
@@ -1562,65 +1672,65 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H15" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H16" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H17" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H18" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H19" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>42</v>
@@ -1628,65 +1738,65 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H21" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H21" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H23" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H24" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H25" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H25" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>42</v>
@@ -1694,65 +1804,65 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H27" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H28" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H29" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H29" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H30" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H30" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H31" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H31" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>42</v>
@@ -1760,65 +1870,65 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="H33" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="H33" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="H34" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="H34" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="H35" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="H35" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="H36" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H36" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="H37" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="H37" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>42</v>
@@ -1826,10 +1936,10 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>42</v>
@@ -1837,65 +1947,65 @@
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="H40" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="H40" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="H41" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="H41" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="H42" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="H42" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="H43" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="H43" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="H44" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="H44" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>42</v>
@@ -1903,65 +2013,65 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="H46" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="H46" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="H47" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="H47" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="H48" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="H48" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="H49" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="H49" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="H50" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="H50" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>42</v>
@@ -1969,10 +2079,10 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="H52" s="0" t="s">
         <v>42</v>
@@ -1997,10 +2107,10 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2170,10 +2280,10 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2235,7 +2345,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.48"/>
   </cols>
@@ -2273,7 +2383,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -2305,7 +2415,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.79"/>
@@ -2329,51 +2439,51 @@
       <c r="B2" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2393,207 +2503,211 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="84.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="6.98"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="6" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="84.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="59.74"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="4" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>80</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>82</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="C2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0"/>
+      <c r="B4" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="D4" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="0"/>
+      <c r="D5" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0"/>
+      <c r="B6" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5"/>
+      <c r="B7" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="0"/>
-      <c r="D3" s="5" t="s">
+      <c r="C8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="0"/>
+      <c r="D9" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="0"/>
+      <c r="D11" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="0"/>
+      <c r="D12" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="0"/>
+      <c r="D13" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5"/>
+      <c r="B14" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5" t="s">
+      <c r="C14" s="0"/>
+      <c r="D14" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="0"/>
-      <c r="D6" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" s="0"/>
-      <c r="D7" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7"/>
-      <c r="B8" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="0"/>
-      <c r="D8" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="0"/>
-      <c r="D9" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="0"/>
-      <c r="D10" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C12" s="0"/>
-      <c r="D12" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C14" s="0"/>
-      <c r="D14" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="0"/>
-      <c r="D15" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" s="0"/>
-      <c r="D16" s="5" t="s">
-        <v>96</v>
+      <c r="C15" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2612,125 +2726,81 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="48.35"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>80</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2740,43 +2810,93 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I33" activeCellId="0" sqref="I33"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="B4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>110</v>
+      <c r="B5" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5"/>
+      <c r="B6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2786,52 +2906,134 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="97.82"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="B4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5"/>
+      <c r="B5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="B6" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="B7" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="B8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="B9" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
+      <c r="B10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Changed topbar color. Added links to Grid. Made projects a menu.
</commit_message>
<xml_diff>
--- a/public/cges/content.xlsx
+++ b/public/cges/content.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="FAQ" sheetId="1" state="visible" r:id="rId2"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="219">
   <si>
     <t xml:space="preserve">Organization:</t>
   </si>
@@ -329,7 +329,6 @@
         <color rgb="FF000000"/>
         <rFont val="padmaa-Bold.1.1"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"</t>
     </r>
@@ -339,7 +338,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+700%</t>
     </r>
@@ -349,7 +347,6 @@
         <color rgb="FF000000"/>
         <rFont val="padmaa-Bold.1.1"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"</t>
     </r>
@@ -394,15 +391,18 @@
     <t xml:space="preserve">Although women are the fastest growing population of incarcerated people, perceptions that they receive preferential treatment from the criminal legal system abound.</t>
   </si>
   <si>
+    <t xml:space="preserve">The CGES Mission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We seek expose intersectional discrimination practices within the criminal legal system and combat extreme sentencing by revealing the contradictions, injustices, and biases of these punishments specifically when used against marginalized populations including women, people of color, transgender individuals, poor people, trauma and abuse survivors, and those with disabilities.</t>
+  </si>
+  <si>
     <t xml:space="preserve">#C6CDF7</t>
   </si>
   <si>
-    <t xml:space="preserve">The CGES Mission</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We seek expose intersectional discrimination practices within the criminal legal system and combat extreme sentencing by revealing the contradictions, injustices, and biases of these punishments specifically when used against marginalized populations including women, people of color, transgender individuals, poor people, trauma and abuse survivors, and those with disabilities.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Our Team</t>
   </si>
   <si>
@@ -509,6 +509,9 @@
   </si>
   <si>
     <t xml:space="preserve">Website Item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cornell.box.com/s/63andrgl6dqxqebmaqq6z6kx1jq7j6c8 https://cornell.box.com/s/rqoakzkph3yxjmcucp3kvvpczuorpl2k</t>
   </si>
   <si>
     <t xml:space="preserve">Organization Item</t>
@@ -732,7 +735,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -754,21 +756,18 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="padmaa-Bold.1.1"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -869,34 +868,34 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="242.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -923,28 +922,28 @@
       <selection pane="topLeft" activeCell="I33" activeCellId="0" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -969,44 +968,44 @@
       <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1031,29 +1030,29 @@
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -1061,22 +1060,22 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>39</v>
@@ -1104,29 +1103,29 @@
       <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -1134,22 +1133,22 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>9</v>
@@ -1157,22 +1156,22 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>12</v>
@@ -1180,22 +1179,22 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>15</v>
@@ -1203,22 +1202,22 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>18</v>
@@ -1226,22 +1225,22 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>21</v>
@@ -1269,29 +1268,29 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -1299,22 +1298,22 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>36</v>
@@ -1322,22 +1321,22 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>33</v>
@@ -1361,108 +1360,114 @@
   </sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="62.24"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>132</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>139</v>
+        <v>24</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>24</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>139</v>
+        <v>30</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>30</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" display="https://cornell.box.com/s/63andrgl6dqxqebmaqq6z6kx1jq7j6c8"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1484,7 +1489,7 @@
       <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.18"/>
   </cols>
@@ -1494,22 +1499,22 @@
         <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -1517,22 +1522,22 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>42</v>
@@ -1540,10 +1545,10 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>42</v>
@@ -1551,10 +1556,10 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>42</v>
@@ -1562,10 +1567,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>155</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>153</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>42</v>
@@ -1573,10 +1578,10 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>42</v>
@@ -1584,10 +1589,10 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>42</v>
@@ -1595,10 +1600,10 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>42</v>
@@ -1606,10 +1611,10 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>42</v>
@@ -1617,10 +1622,10 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>159</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>42</v>
@@ -1628,10 +1633,10 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>42</v>
@@ -1639,10 +1644,10 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>42</v>
@@ -1650,10 +1655,10 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>165</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>163</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>42</v>
@@ -1661,10 +1666,10 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>42</v>
@@ -1672,10 +1677,10 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>42</v>
@@ -1683,10 +1688,10 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>42</v>
@@ -1694,10 +1699,10 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>42</v>
@@ -1705,10 +1710,10 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>42</v>
@@ -1716,10 +1721,10 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>42</v>
@@ -1727,10 +1732,10 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>42</v>
@@ -1738,10 +1743,10 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>42</v>
@@ -1749,10 +1754,10 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>42</v>
@@ -1760,10 +1765,10 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>42</v>
@@ -1771,10 +1776,10 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>42</v>
@@ -1782,10 +1787,10 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>42</v>
@@ -1793,10 +1798,10 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>42</v>
@@ -1804,10 +1809,10 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>42</v>
@@ -1815,10 +1820,10 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>42</v>
@@ -1826,10 +1831,10 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>42</v>
@@ -1837,10 +1842,10 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>42</v>
@@ -1848,10 +1853,10 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>42</v>
@@ -1859,10 +1864,10 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>42</v>
@@ -1870,10 +1875,10 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>42</v>
@@ -1881,10 +1886,10 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>42</v>
@@ -1892,10 +1897,10 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B35" s="0" t="s">
         <v>188</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>186</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>42</v>
@@ -1903,10 +1908,10 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>42</v>
@@ -1914,10 +1919,10 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>42</v>
@@ -1925,10 +1930,10 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>42</v>
@@ -1936,10 +1941,10 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>42</v>
@@ -1947,10 +1952,10 @@
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>42</v>
@@ -1958,10 +1963,10 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>42</v>
@@ -1969,10 +1974,10 @@
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>42</v>
@@ -1980,10 +1985,10 @@
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H43" s="3" t="s">
         <v>42</v>
@@ -1991,10 +1996,10 @@
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>42</v>
@@ -2002,10 +2007,10 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>42</v>
@@ -2013,10 +2018,10 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>42</v>
@@ -2024,10 +2029,10 @@
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H47" s="3" t="s">
         <v>42</v>
@@ -2035,10 +2040,10 @@
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>42</v>
@@ -2046,10 +2051,10 @@
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="B49" s="0" t="s">
         <v>213</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>211</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>42</v>
@@ -2057,10 +2062,10 @@
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>42</v>
@@ -2068,10 +2073,10 @@
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>42</v>
@@ -2079,10 +2084,10 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H52" s="0" t="s">
         <v>42</v>
@@ -2110,7 +2115,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2280,7 +2285,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.82"/>
@@ -2345,7 +2350,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.48"/>
   </cols>
@@ -2390,7 +2395,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
     </row>
   </sheetData>
@@ -2415,13 +2420,13 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.79"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
@@ -2908,11 +2913,11 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="97.82"/>
   </cols>
@@ -2939,23 +2944,23 @@
         <v>84</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2965,8 +2970,11 @@
       <c r="B4" s="4" t="s">
         <v>97</v>
       </c>
+      <c r="C4" s="0" t="s">
+        <v>85</v>
+      </c>
       <c r="D4" s="4" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2975,12 +2983,12 @@
         <v>84</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>62</v>
@@ -2991,46 +2999,46 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>97</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>97</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Added li components & content
</commit_message>
<xml_diff>
--- a/public/cges/content.xlsx
+++ b/public/cges/content.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="FAQ" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Card Types" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Card Types" sheetId="2" state="hidden" r:id="rId3"/>
     <sheet name="Main Categories" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Projects Categories" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Carousel" sheetId="5" state="visible" r:id="rId6"/>
@@ -17,13 +17,17 @@
     <sheet name="Landing Image Example" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Landing Parallax Example" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="About" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Women on Death Row" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Women on Death Row Categories" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Women on Death Row Categories" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Fellows List" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="Fellows Cards" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Toolkit Cards" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="News &amp; Events Cards" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="Resource Hub Cards" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="Women on Death Row Cards" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="Toolkit List" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Toolkit Cards" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="News &amp; Events List" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="News &amp; Events Cards" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="Resource Hub List" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="Resource Hub Cards" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="Women on Death Row List" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="Women on Death Row Cards" sheetId="20" state="visible" r:id="rId21"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="231">
   <si>
     <t xml:space="preserve">Organization:</t>
   </si>
@@ -50,7 +54,7 @@
     <t xml:space="preserve">All Narrative sheets will contain long form narrative info</t>
   </si>
   <si>
-    <t xml:space="preserve">Every card type and assoicated color will be in the types sheet</t>
+    <t xml:space="preserve">Every card type and associated color will be in the types sheet</t>
   </si>
   <si>
     <t xml:space="preserve">Cards on the website will be ordered by their row in the respective Content sheet</t>
@@ -290,22 +294,22 @@
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
+    <t xml:space="preserve">Landing Image Example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bg-image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">landingimg.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content contained in landing image example sheet </t>
+  </si>
+  <si>
     <t xml:space="preserve">space</t>
   </si>
   <si>
     <t xml:space="preserve">white</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Landing Image Example</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bg-image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">landingimg.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Content contained in landing image example sheet </t>
   </si>
   <si>
     <t xml:space="preserve">Landing Parallax Example</t>
@@ -329,6 +333,7 @@
         <color rgb="FF000000"/>
         <rFont val="padmaa-Bold.1.1"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"</t>
     </r>
@@ -338,6 +343,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+700%</t>
     </r>
@@ -347,6 +353,7 @@
         <color rgb="FF000000"/>
         <rFont val="padmaa-Bold.1.1"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"</t>
     </r>
@@ -391,78 +398,93 @@
     <t xml:space="preserve">Although women are the fastest growing population of incarcerated people, perceptions that they receive preferential treatment from the criminal legal system abound.</t>
   </si>
   <si>
-    <t xml:space="preserve">The CGES Mission</t>
-  </si>
-  <si>
-    <t xml:space="preserve">black</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We seek expose intersectional discrimination practices within the criminal legal system and combat extreme sentencing by revealing the contradictions, injustices, and biases of these punishments specifically when used against marginalized populations including women, people of color, transgender individuals, poor people, trauma and abuse survivors, and those with disabilities.</t>
-  </si>
-  <si>
     <t xml:space="preserve">#C6CDF7</t>
   </si>
   <si>
-    <t xml:space="preserve">Our Team</t>
+    <t xml:space="preserve">The Center on Gender and Extreme Sentencing was founded in response to the exclusion of women, particularly women of color, from conversations surrounding mass incarceration in the United States. For too long, women, trans folks, and gender minorities have been left behind by researchers, advocates, and impact litigation efforts. This exclusion exists for multiple reasons, including the sense that because there are comparatively fewer women behind bars, that efforts would be better spent studying, advocating for, and litigating on behalf of incarcerated men. However, women’s incarceration rates are growing faster than those of men. As of 2023, the population of incarcerated women in the United States was six times higher than in 1980 (The Sentencing Project, 2023). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Women are also left out of discussions around the criminal legal system because of societal gender bias and institutionalized misogyny. We see this reflected in the stories of our clients, many of whom were ignored and disregarded when they were victims of crimes, then villainized and criminalized when they became perpetrators. The normalization of gender-based violence and misogyny means that many women’s experiences of gender-based oppression and violence are marginalized and minimized before the juries that condemned them to extreme punishments. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We know from years of experience defending women and gender minorities accused of serious crimes that their lives, experiences, and paths to incarceration are fundamentally different from those of men. So too are their experiences within prison systems designed to house men. Our goal at CGES is to uplift these stories, while bolstering them with rigorous research and advocacy that challenges how women have been treated by the criminal legal system. We seek to leverage systemic change within the criminal legal system by advocating for and beside the most marginalized members of our community who are incarcerated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our work addresses intersectional discrimination from a variety of angles. We shed light on hidden forms of discrimination and disrupt widespread misconceptions about its prevalence. We engage in advocacy campaigning to inform the public and mobilize new allies for change. We produce materials of practical relevance for lawyers, policy-makers, and most importantly, incarcerated people.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our Team:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are a multidisciplinary group of lawyers, human rights defenders, scholars, experts, and researchers dedicated to exposing the intersectional bias faced by women, trans people, and gender minorities facing extreme sentencing. We engage in advocacy and research, and share practical resources with advocates and people who have directly experienced incarceration, with the goal of effecting systemic change within the criminal legal system. By focusing on the most vulnerable members of the incarcerated population, we believe our approach will gain victories that will be felt throughout the prison industrial complex, to the benefit of all people subjected to the harms of mass incarceration.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kwaneta Harris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kwaneta Harris is a former nurse, business owner and expat, now incarcerated journalist and a Haymarket Writing Freedom Fellow. She brings experiences from each profession to illuminate how the experience of being incarcerated in the largest state prison in Texas is vastly different for women in ways that directly map onto a culture rooted in misogyny. Her powerful and shocking stories expose how the intersection of gender, race and place contribute to state-sanctioned, gender-based violence. As an advisory board member of CGES, Kwaneta’s input is an invaluable asset towards ensuring our programming is responsive to the needs of incarcerated women. You can read Kwaneta’s writing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ch.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bahar Mirhosseni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bahar Mirhosseni is a human rights advocate, a criminal defense lawyer, and the Director of Legal Advocacy at the Cornell Center on the Death Penalty Worldwide. She also co-teaches the Pretrial Justice Clinic at UCLA School of Law. She has collaborated with a range of human rights organizations including the Georgia Capital Defender Office, the Southern Africa Litigation Centre, and Addameer Prisoner Support and Human Rights Association. She serves on both the Racial Justice Committee and the Education Committee of the National Association for Public Defense. She has spent over sixteen years in indigent defense, as a public defender in New York and California, and in partnership with public defenders overseas, on access to justice, human rights, and high quality lawyering.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chelsea Halstead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chelsea Halstead is the Director of the Cornell Center on the Death Penalty Worldwide, where she oversees the center’s operations, communications, strategy, advocacy, and fundraising efforts. Prior to her appointment at CCDPW, Chelsea co-founded the Colibrí Center for Human Rights in Tucson, Arizona. Colibrí combines forensic science with human rights advocacy to identify the remains of people who have died in their attempt to cross the U.S.-Mexico border while calling attention to failed immigration policy. Chelsea helped design the organization’s innovative DNA program, which has facilitated the identification of over 200 previously unidentified human remains. Her work has been recognized in USA Today, The Guardian, The New York Times, The Washington Post, Al Jazeera, and other media. Chelsea holds a B.A. in Geography from the University of Arizona and an M.P.A. from Cornell University.</t>
   </si>
   <si>
     <t xml:space="preserve">Sandra Babcock</t>
   </si>
   <si>
-    <t xml:space="preserve">sb.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chelsea Halsead</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ch.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">image</t>
+    <t xml:space="preserve">Sandra Babcock is a Clinical Professor at Cornell Law School, where she is the Faculty Director and founder of the Cornell Center on the Death Penalty Worldwide (CCDPW). Over the last thirty years she has helped defend hundreds of men and women facing execution around the world. She began her career as a staff attorney at the Texas Resource Center, where she defended persons facing execution in post-conviction proceedings for four years. Following a five-year stint as a public defender in Minneapolis, she served for six years as the founding director of the Mexican Capital Legal Assistance Program, a project funded by the Government of Mexico to defend Mexican nationals facing the death penalty in the U.S. In that capacity she provided litigation support to attorneys around the country, defended Mexican nationals facing execution, and represented Mexico before the International Court of Justice in Avena and Other Mexican Nationals. In 2006, she became a Clinical Professor at Northwestern Law School, where she spearheaded a ten-year project in Malawi that ultimately resulted in the release of over 250 prisoners, 150 of whom were formerly sentenced to death. She moved to Cornell Law in 2014, where she founded the Cornell Center on the Death Penalty Worldwide. In 2018, together with her colleagues at CDPW, she launched the Alice Project, a global movement to end extreme sentencing of women and gender non-conforming individuals. Her clinic currently represents women facing the death penalty in the United States, Malawi, and Tanzania. She has authored numerous articles, book chapters and reports on the application of the death penalty under international law. She teaches classes in international human rights, gender rights, and the death penalty. In September 2021, she received the American Bar Association’s John Paul Stevens Guiding Hand of Counsel Award, given to one capital defender every two years whose work has improved the legal representation of persons facing the death penalty and contributed to systemic reform.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conditions of Detention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each of these need their own content sheet if they are containers for cards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transwomen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intersectional Bias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender-Based Violence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mental Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discrimination in the Legal System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fellows:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In recognition of the expertise that formerly incarcerated people have gained through their lived experience, we have created the Future Freedoms Fellowship. This program provides a part time stipend and a small pool of career development funding to professionals who are interested in social justice advocacy and criminal legal system reform. Our goal is to provide returning community members with financial support, professional development opportunities, speaking engagements, advocacy training, and other tools to assist them with rebuilding careers after incarceration. Our fellows bring expertise to guide us in ensuring our organizational programming reflects the needs and desires of people who are still incarcerated. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">subtitle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abstract_image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abstract</t>
   </si>
   <si>
     <t xml:space="preserve">body</t>
   </si>
   <si>
-    <t xml:space="preserve">mytitle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">person img</t>
-  </si>
-  <si>
-    <t xml:space="preserve">their story</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conditions of Detention</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Each of these need their own content sheet if they are containers for cards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transwomen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intersectional Bias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gender-Based Violence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mental Health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Discrimination in the Legal System</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subtitle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abstract_image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abstract</t>
-  </si>
-  <si>
     <t xml:space="preserve">attachments</t>
   </si>
   <si>
@@ -487,6 +509,15 @@
     <t xml:space="preserve">PDFs</t>
   </si>
   <si>
+    <t xml:space="preserve">Test Content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toolkit:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here you will find sample legal briefs, clemency petitions, resources on narrative construction, litigation manuals, and factsheets relating to the defense of women and gender minorities on the following key issues: gender-based violence, sex trafficking, coercive control, trauma, mental health, intersectional discrimination, prison conditions, and working with the media. The materials in our toolkit are free and easily accessible, with the vision that equipping diverse defense communities with these resources will advance advocacy on behalf of criminalized women, transgender people, and gender minorities.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brief Item</t>
   </si>
   <si>
@@ -508,12 +539,18 @@
     <t xml:space="preserve">Event Item</t>
   </si>
   <si>
+    <t xml:space="preserve">Resource Hub:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our resource hub is designed for legal teams, advocates, and scholars interested in women facing extreme punishment. It includes information on (1) women’s pathways to incarceration, with particular focus on violence against women; (2) conditions of detention; (3) harmful gender stereotypes; and (4) intersectional discrimination. Additionally, we have compiled a library of resources on a variety of topics relating to the defense of women and gender minorities, which we can make available to advocates who sign up at the portal below. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAILSIGNUPHERE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Website Item</t>
   </si>
   <si>
-    <t xml:space="preserve">https://cornell.box.com/s/63andrgl6dqxqebmaqq6z6kx1jq7j6c8 https://cornell.box.com/s/rqoakzkph3yxjmcucp3kvvpczuorpl2k</t>
-  </si>
-  <si>
     <t xml:space="preserve">Organization Item</t>
   </si>
   <si>
@@ -521,6 +558,12 @@
   </si>
   <si>
     <t xml:space="preserve">Report Item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Women on Death Row: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currently, there is a dearth of publicly accessible, reliable information on women sentenced to death around the world. We are committed to publishing data and research that increases knowledge about incarcerated women and their experiences. At the same time, we recognize that many incarcerated women do not wish to be publicly identified, and we believe in giving them control over how their stories are shared. For this reason, we do not share the names of people on death row or any information about their cases unless they or their legal representatives have given us express permission to do so. Where we receive that permission, we will share information on advocacy campaigns for women at risk of execution. We will also share anonymized data and studies that can assist in broadening awareness about the intersection of gender and the death penalty. </t>
   </si>
   <si>
     <t xml:space="preserve">Case Item</t>
@@ -729,12 +772,13 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -756,11 +800,30 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="padmaa-Bold.1.1"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="0"/>
     </font>
     <font>
@@ -768,6 +831,7 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -812,7 +876,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -841,7 +905,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -865,37 +941,37 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="242.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -916,34 +992,50 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I33" activeCellId="0" sqref="I33"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -962,59 +1054,78 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>129</v>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1030,29 +1141,29 @@
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -1060,22 +1171,22 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>39</v>
@@ -1097,162 +1208,112 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.62"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>21</v>
+      <c r="C3" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1262,35 +1323,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -1298,48 +1359,117 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1358,116 +1488,110 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="62.24"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>145</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>149</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>140</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="https://cornell.box.com/s/63andrgl6dqxqebmaqq6z6kx1jq7j6c8"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1478,621 +1602,445 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="C3" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="A4" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="A6" s="5"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="A7" s="5"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="A8" s="5"/>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="H26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="H32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="H38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="H39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="H45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="H50" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="B52" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="H52" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2115,7 +2063,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2261,6 +2209,632 @@
       </c>
       <c r="C13" s="3" t="s">
         <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H52"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.18"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="H52" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2285,7 +2859,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.82"/>
@@ -2350,7 +2924,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.48"/>
   </cols>
@@ -2395,7 +2969,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
     </row>
   </sheetData>
@@ -2420,13 +2994,13 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.79"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
@@ -2508,10 +3082,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2542,125 +3116,126 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>84</v>
+      </c>
       <c r="B2" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="C2" s="0"/>
       <c r="D2" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>86</v>
-      </c>
+      <c r="A3" s="0"/>
       <c r="B3" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" s="0"/>
+        <v>88</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>89</v>
+      </c>
       <c r="D3" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="0"/>
+      <c r="D4" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0"/>
+      <c r="B5" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="C5" s="0" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0"/>
-      <c r="B4" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="C5" s="0"/>
       <c r="D5" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0"/>
-      <c r="B6" s="0" t="s">
-        <v>84</v>
+      <c r="A6" s="5"/>
+      <c r="B6" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
+        <v>89</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>95</v>
+      </c>
       <c r="B7" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>85</v>
+        <v>62</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
-        <v>95</v>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>85</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C8" s="0"/>
       <c r="D8" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>96</v>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9" s="0"/>
+        <v>62</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="D9" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>98</v>
+    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>85</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C10" s="0"/>
       <c r="D10" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>97</v>
@@ -2670,9 +3245,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>97</v>
@@ -2682,12 +3257,10 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>101</v>
-      </c>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5"/>
       <c r="B13" s="4" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C13" s="0"/>
       <c r="D13" s="4" t="s">
@@ -2695,24 +3268,14 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5"/>
-      <c r="B14" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="0"/>
-      <c r="D14" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>85</v>
+      <c r="B14" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2737,7 +3300,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="48.35"/>
   </cols>
@@ -2759,7 +3322,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
@@ -2786,13 +3349,13 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
@@ -2821,7 +3384,7 @@
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
   </cols>
@@ -2843,7 +3406,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
@@ -2858,7 +3421,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>102</v>
@@ -2872,7 +3435,7 @@
         <v>62</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2883,13 +3446,13 @@
         <v>97</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5"/>
       <c r="B6" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>102</v>
@@ -2913,13 +3476,13 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="97.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2941,104 +3504,278 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>109</v>
+        <v>47</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>111</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>85</v>
-      </c>
       <c r="D4" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="B6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5"/>
+      <c r="B8" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5"/>
+      <c r="B9" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="B7" s="0" t="s">
+      <c r="D10" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="D11" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5"/>
+      <c r="B12" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="B9" s="0" t="s">
+      <c r="D15" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5"/>
+      <c r="B16" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="D18" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>112</v>
+      <c r="D19" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5"/>
+      <c r="B20" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5"/>
+      <c r="B24" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Revisions from last meeting.  First map.
</commit_message>
<xml_diff>
--- a/public/cges/content.xlsx
+++ b/public/cges/content.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="15"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Card Types" sheetId="1" state="hidden" r:id="rId2"/>
@@ -27,6 +27,7 @@
     <sheet name="Resource Hub Cards" sheetId="17" state="visible" r:id="rId18"/>
     <sheet name="Women on Death Row List" sheetId="18" state="visible" r:id="rId19"/>
     <sheet name="Women on Death Row Cards" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="WODR Map" sheetId="20" state="visible" r:id="rId21"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="424">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -429,6 +430,56 @@
     <t xml:space="preserve">babcock.jpg</t>
   </si>
   <si>
+    <t xml:space="preserve">Dorian Bess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dorian Bess brings a wealth of knowledge and experience to her role
+as the Program Development and Engagement Officer of The Social
+Justice Network. With 18 years of lived experience within the Criminal
+Justice System, she has transformed her journey into a career
+dedicated to supporting justice-impacted individuals through reentry
+services, mental health advocacy, and specialized care for women
+experiencing trauma and substance abuse.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dorian's professional background includes her impactful work with the Department of Health
+and Mental Hygiene, where she served as a Community Health Worker focusing on reentry
+services for citizens returning from city, state, and federal facilities.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Her hands-on experience in navigating the complexities of reentry has made her a key player in
+helping individuals rebuild their lives post-incarceration. In addition to her reentry work, Dorian
+plays an active role in the National Action Network's Second Chance Committee, where she
+collaborates with the crisis and prevention team to address the needs of justice-impacted
+Communities.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Her dedication to this cause is further demonstrated by her ability to foster strong partnerships
+with local groups, as well as state and federal agencies, to create and implement programs that
+address education, mental health, substance use, and reentry challenges. Dorian is not just a
+leader but also a connector, known for her ability to build robust internal networks that drive
+meaningful change. Her work emphasizes the importance of communication and leadership in
+advancing initiatives that aim for systemic reform.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Through her efforts, she continuously creates spaces for crucial conversations that pave the
+way for genuine reform within the criminal justice system. Dorian’s commitment to her work and
+her community is evident in everything she does, making her an invaluable asset to the Social
+Justice Network and a beacon of hope for those she serves.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dorian.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Johdy Polk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jhody Polk, d’Alchemist, is the founder of the Jailhouse Lawyers Initiative (JLI) housed at the Bernstein Institute for Human Rights at NYU School of Law and she is the founder of the Legal Empowerment &amp; Advocacy Hub (LEAH). Jhody is a 2024 Global Freedom Fellow and an inaugural 2024 Future Freedoms Fellow with the Center on Gender and Extreme Sentencing. Jhody is the recipient of the 2019 Peacebuilder of the Year Award, the 2020 Dr. Martin Luther King’s Jr. Legacy award and named a Soros Justice Fellow in 2018. She currently serves on the Board of Namati. Jhody is known for her work as a central Florida Organizer on Amendment 4 which restored the right to vote to over a million Floridians with felony convictions. She was the 2023 Legal Empowerment Fellow of the Global Justice Clinic at NYU Law School, the 2023 inaugural Pathways to Research and Advocacy Fellow with the Fortune Society and Center for Justice Innovation and the former Director of Community Justice at the River Phoenix Center for Peacebuilding. Jhody also served 3 years as the Director of the Alachua County Reentry Coalition in her hometown of Gainesville, Florida. During her incarceration Jhody gained her legal identity and became a teacher, translator and facilitator of the law as a jailhouse lawyer working in the prison law library. d’Alchemist describes herself as “Justice Living” not "justice impacted. She uses her work and life to accelerate SDG16 and to establish legal empowerment as a proactive tool of abolition in the US.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">johdy.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fellows:</t>
   </si>
   <si>
@@ -477,7 +528,10 @@
     <t xml:space="preserve">Here you will find sample legal briefs, clemency petitions, resources on narrative construction, litigation manuals, and factsheets relating to the defense of women and gender minorities on the following key issues: gender-based violence, sex trafficking, coercive control, trauma, mental health, intersectional discrimination, prison conditions, and working with the media. The materials in our toolkit are free and easily accessible, with the vision that equipping diverse defense communities with these resources will advance advocacy on behalf of criminalized women, transgender people, and gender minorities.</t>
   </si>
   <si>
-    <t xml:space="preserve">Manual Item</t>
+    <t xml:space="preserve">Defending Women and Transgender Persons - ADA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defending Women and Transgender Persons - ADA.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Manuals</t>
@@ -489,13 +543,19 @@
     <t xml:space="preserve">Factsheets</t>
   </si>
   <si>
-    <t xml:space="preserve">CM Item</t>
+    <t xml:space="preserve">Melissa Lucio - Clemency Petition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melissa Lucio - Clemency Petition.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Clemency Materials</t>
   </si>
   <si>
-    <t xml:space="preserve">LT Item</t>
+    <t xml:space="preserve">Lisa Montgomery - Petition to the Inter-American Commission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lisa Montgomery - Petition to the Inter-American Commission.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Litigation Tools</t>
@@ -511,6 +571,18 @@
   </si>
   <si>
     <t xml:space="preserve">Sign up for Resource Hub Access</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;iframe
+    src="/cges/mailchimp.html"
+    style="
+      width: 100%;
+      height: 350px;
+      border: none;
+      box-shadow: none;
+      overflow: hidden;
+    "
+  /&gt;</t>
   </si>
   <si>
     <r>
@@ -528,6 +600,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">&lt;a href='/cges/resources' target='_blank' rel='noopener' &gt; here &lt;/a&gt;</t>
     </r>
@@ -542,19 +615,55 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">B Item</t>
+    <t xml:space="preserve">Gender and Extreme Sentencing of Women </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Bibliography </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">8-14-24</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Bibliography - Gender and Extreme Sentencing of Women 8-14-2024.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Bibliography</t>
   </si>
   <si>
-    <t xml:space="preserve">R Item</t>
+    <t xml:space="preserve">Judged for More Than Her Crime_low-res </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"08-30-23"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Judged for More Than Her Crime_low-res 2018-08-30.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Reports</t>
   </si>
   <si>
-    <t xml:space="preserve">AA Item</t>
+    <t xml:space="preserve">Babcock and Greenfield - Gender, Violence, and DP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06-13-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Babcock and Greenfield - Gender, Violence, and DP - 6-13-23.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Academic Articles</t>
@@ -762,17 +871,561 @@
   </si>
   <si>
     <t xml:space="preserve">Kimberly Cargill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WODR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afghanistan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Murder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algeria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antigua and Barbuda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bahamas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bahrain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bangladesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barbados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belarus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Botswana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brunei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cameroon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Murder, unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comoros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Democratic Republic of the Congo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dominica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egypt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Murder, storming government installations, terrorism, espionage, rape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eritrea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethiopia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gambia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grenada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guyana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indonesia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Murder, drug offenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Many</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iraq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Murder, terrorism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jamaica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Japan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aggravated murder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jordan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kenya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100-200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kuwait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug offense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lebanon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lesotho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liberia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Libya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malawi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malaysia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maldives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adultery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mauritania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morocco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Myanmar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nigeria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Korea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknown/many</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pakistan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palestine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qatar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At least 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saint Kitts and Nevis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saint Lucia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saint Vincent and the Grenadines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saudi Arabia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Murder, drug offenses, sorcery, witchcraft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Singapore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Several</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug offenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somalia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Korea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Sudan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">at least 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sri Lanka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sudan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Many/unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Murder, adultery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Syria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taiwan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tajikistan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tanzania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">at least 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thailand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tonga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trinidad and Tobago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tunisia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uganda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Arab Emirates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">at least  1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vietnam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">at least 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drug offenses, financial fraud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yemen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Murder, aiding an enemy country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zimbabwe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -801,12 +1454,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -840,6 +1487,33 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -885,7 +1559,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -906,19 +1580,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -926,12 +1600,36 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -957,7 +1655,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1127,7 +1825,7 @@
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -1153,8 +1851,8 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>120</v>
+      <c r="A3" s="9" t="s">
+        <v>130</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>53</v>
@@ -1167,8 +1865,8 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
-        <v>121</v>
+      <c r="A4" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>80</v>
@@ -1178,7 +1876,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="4" t="s">
         <v>75</v>
       </c>
@@ -1217,29 +1915,29 @@
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -1247,22 +1945,22 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>33</v>
@@ -1290,7 +1988,7 @@
       <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.27"/>
@@ -1320,8 +2018,8 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>134</v>
+      <c r="A3" s="9" t="s">
+        <v>144</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>53</v>
@@ -1334,8 +2032,8 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
-        <v>135</v>
+      <c r="A4" s="9" t="s">
+        <v>145</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>80</v>
@@ -1345,7 +2043,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="4" t="s">
         <v>75</v>
       </c>
@@ -1378,130 +2076,107 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>129</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>129</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>129</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1511,7 +2186,6 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="H6" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1535,7 +2209,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1558,29 +2232,29 @@
       <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -1588,22 +2262,22 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>30</v>
@@ -1634,13 +2308,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.1"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -1666,8 +2343,8 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>145</v>
+      <c r="A3" s="9" t="s">
+        <v>158</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>53</v>
@@ -1680,8 +2357,8 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
-        <v>146</v>
+      <c r="A4" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>80</v>
@@ -1692,7 +2369,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>53</v>
@@ -1701,41 +2378,52 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10"/>
+    <row r="6" customFormat="false" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12" t="s">
+        <v>161</v>
+      </c>
       <c r="B6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9"/>
+      <c r="B7" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
+      <c r="A8" s="9" t="s">
+        <v>162</v>
+      </c>
       <c r="B8" s="4" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1755,107 +2443,97 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="65.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="63.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>129</v>
+        <v>164</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>150</v>
+        <v>165</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>129</v>
+        <v>167</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>168</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>152</v>
+        <v>169</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>129</v>
+        <v>171</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>172</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>154</v>
+        <v>141</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1880,7 +2558,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.18"/>
   </cols>
@@ -1916,8 +2594,8 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>155</v>
+      <c r="A3" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>53</v>
@@ -1931,8 +2609,8 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
-        <v>156</v>
+      <c r="A4" s="9" t="s">
+        <v>176</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>80</v>
@@ -1943,7 +2621,7 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="4" t="s">
         <v>75</v>
       </c>
@@ -1963,11 +2641,11 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
+      <c r="A7" s="5"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
+      <c r="A8" s="5"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2119,10 +2797,10 @@
   <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.18"/>
   </cols>
@@ -2132,22 +2810,22 @@
         <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -2155,88 +2833,88 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>158</v>
+      <c r="A3" s="5" t="s">
+        <v>178</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>160</v>
+      <c r="A4" s="5" t="s">
+        <v>180</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>161</v>
+      <c r="A5" s="5" t="s">
+        <v>181</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
-        <v>162</v>
+      <c r="A6" s="5" t="s">
+        <v>182</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>163</v>
+      <c r="A7" s="5" t="s">
+        <v>183</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
-        <v>164</v>
+      <c r="A8" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>36</v>
@@ -2244,10 +2922,10 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>36</v>
@@ -2255,10 +2933,10 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>36</v>
@@ -2266,10 +2944,10 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>36</v>
@@ -2277,10 +2955,10 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>36</v>
@@ -2288,10 +2966,10 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>36</v>
@@ -2299,10 +2977,10 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>36</v>
@@ -2310,10 +2988,10 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>36</v>
@@ -2321,10 +2999,10 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>36</v>
@@ -2332,10 +3010,10 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>36</v>
@@ -2343,10 +3021,10 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>36</v>
@@ -2354,10 +3032,10 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>36</v>
@@ -2365,10 +3043,10 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>36</v>
@@ -2376,10 +3054,10 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>36</v>
@@ -2387,10 +3065,10 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>36</v>
@@ -2398,10 +3076,10 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>36</v>
@@ -2409,10 +3087,10 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>36</v>
@@ -2420,10 +3098,10 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>36</v>
@@ -2431,10 +3109,10 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>36</v>
@@ -2442,10 +3120,10 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>36</v>
@@ -2453,10 +3131,10 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>36</v>
@@ -2464,10 +3142,10 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>36</v>
@@ -2475,10 +3153,10 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>36</v>
@@ -2486,10 +3164,10 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="B31" s="0" t="s">
         <v>189</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>169</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>36</v>
@@ -2497,10 +3175,10 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>36</v>
@@ -2508,10 +3186,10 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>36</v>
@@ -2519,10 +3197,10 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>36</v>
@@ -2530,10 +3208,10 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>36</v>
@@ -2541,10 +3219,10 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>36</v>
@@ -2552,10 +3230,10 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>36</v>
@@ -2563,10 +3241,10 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>36</v>
@@ -2574,10 +3252,10 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>36</v>
@@ -2585,10 +3263,10 @@
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>36</v>
@@ -2596,10 +3274,10 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>36</v>
@@ -2607,10 +3285,10 @@
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>36</v>
@@ -2618,10 +3296,10 @@
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>36</v>
@@ -2629,10 +3307,10 @@
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>36</v>
@@ -2640,10 +3318,10 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>36</v>
@@ -2651,10 +3329,10 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>36</v>
@@ -2662,10 +3340,10 @@
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>36</v>
@@ -2673,10 +3351,10 @@
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>36</v>
@@ -2684,10 +3362,10 @@
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>36</v>
@@ -2695,10 +3373,10 @@
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>36</v>
@@ -2706,10 +3384,10 @@
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>36</v>
@@ -2717,10 +3395,10 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="H52" s="0" t="s">
         <v>36</v>
@@ -2748,7 +3426,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.82"/>
@@ -2798,6 +3476,997 @@
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D77"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="16" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="16" width="27.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="16" width="22.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="16" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="C2" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="C4" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="C5" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="C6" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="C7" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="C8" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="C9" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="C11" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="C12" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="C13" s="16" t="n">
+        <v>14</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="C14" s="16" t="n">
+        <v>56</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="C15" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="C16" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="C17" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="C18" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="16" t="s">
+        <v>284</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>285</v>
+      </c>
+      <c r="C19" s="16" t="n">
+        <v>146</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="C20" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="16" t="s">
+        <v>289</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="C21" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="C22" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="16" t="s">
+        <v>293</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>294</v>
+      </c>
+      <c r="C23" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="16" t="s">
+        <v>295</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="C24" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="16" t="s">
+        <v>297</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>298</v>
+      </c>
+      <c r="C25" s="16" t="n">
+        <v>12</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="C26" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>303</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="16" t="s">
+        <v>305</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>307</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="16" t="s">
+        <v>309</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>310</v>
+      </c>
+      <c r="C29" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="16" t="s">
+        <v>311</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>312</v>
+      </c>
+      <c r="C30" s="16" t="n">
+        <v>7</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>315</v>
+      </c>
+      <c r="C31" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="16" t="s">
+        <v>316</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>317</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="16" t="s">
+        <v>319</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="C33" s="16" t="n">
+        <v>6</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="16" t="s">
+        <v>321</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>322</v>
+      </c>
+      <c r="C34" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>325</v>
+      </c>
+      <c r="C35" s="16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="16" t="s">
+        <v>326</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>327</v>
+      </c>
+      <c r="C36" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="16" t="s">
+        <v>328</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>329</v>
+      </c>
+      <c r="C37" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="16" t="s">
+        <v>330</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>331</v>
+      </c>
+      <c r="C38" s="16" t="n">
+        <v>3</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="16" t="s">
+        <v>332</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>333</v>
+      </c>
+      <c r="C39" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="16" t="s">
+        <v>334</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>335</v>
+      </c>
+      <c r="C40" s="16" t="n">
+        <v>143</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="16" t="s">
+        <v>336</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>337</v>
+      </c>
+      <c r="C41" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="16" t="s">
+        <v>339</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="C42" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="16" t="s">
+        <v>341</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>342</v>
+      </c>
+      <c r="C43" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="C44" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="16" t="s">
+        <v>345</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>346</v>
+      </c>
+      <c r="C45" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>348</v>
+      </c>
+      <c r="C46" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="16" t="s">
+        <v>349</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="C47" s="16" t="n">
+        <v>32</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="16" t="s">
+        <v>351</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>352</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>353</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="16" t="s">
+        <v>354</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>355</v>
+      </c>
+      <c r="C49" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="16" t="s">
+        <v>356</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>357</v>
+      </c>
+      <c r="C50" s="16" t="n">
+        <v>29</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="16" t="s">
+        <v>358</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>359</v>
+      </c>
+      <c r="C51" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="16" t="s">
+        <v>363</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>364</v>
+      </c>
+      <c r="C53" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="16" t="s">
+        <v>365</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="C54" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>368</v>
+      </c>
+      <c r="C55" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="16" t="s">
+        <v>369</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>370</v>
+      </c>
+      <c r="C56" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="16" t="s">
+        <v>371</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>372</v>
+      </c>
+      <c r="C57" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="D57" s="16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="16" t="s">
+        <v>374</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>376</v>
+      </c>
+      <c r="D58" s="16" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="16" t="s">
+        <v>380</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="C60" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="16" t="s">
+        <v>382</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>383</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>384</v>
+      </c>
+      <c r="D61" s="16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="16" t="s">
+        <v>385</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>386</v>
+      </c>
+      <c r="C62" s="16" t="n">
+        <v>84</v>
+      </c>
+      <c r="D62" s="16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="16" t="s">
+        <v>387</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="D63" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="16" t="s">
+        <v>391</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>392</v>
+      </c>
+      <c r="C64" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="16" t="s">
+        <v>393</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>394</v>
+      </c>
+      <c r="C65" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D65" s="16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="16" t="s">
+        <v>395</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="C66" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="16" t="s">
+        <v>397</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>398</v>
+      </c>
+      <c r="C67" s="16" t="s">
+        <v>399</v>
+      </c>
+      <c r="D67" s="16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="16" t="s">
+        <v>400</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>401</v>
+      </c>
+      <c r="C68" s="16" t="n">
+        <v>33</v>
+      </c>
+      <c r="D68" s="16" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="16" t="s">
+        <v>402</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>403</v>
+      </c>
+      <c r="C69" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>405</v>
+      </c>
+      <c r="C70" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D70" s="16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="16" t="s">
+        <v>406</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>407</v>
+      </c>
+      <c r="C71" s="16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="16" t="s">
+        <v>408</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>409</v>
+      </c>
+      <c r="C72" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="D72" s="16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>411</v>
+      </c>
+      <c r="C73" s="16" t="s">
+        <v>412</v>
+      </c>
+      <c r="D73" s="16" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="16" t="s">
+        <v>413</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>414</v>
+      </c>
+      <c r="C74" s="16" t="n">
+        <v>52</v>
+      </c>
+      <c r="D74" s="16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="B75" s="16" t="s">
+        <v>416</v>
+      </c>
+      <c r="C75" s="16" t="s">
+        <v>417</v>
+      </c>
+      <c r="D75" s="16" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="16" t="s">
+        <v>419</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>420</v>
+      </c>
+      <c r="C76" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D76" s="16" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="16" t="s">
+        <v>422</v>
+      </c>
+      <c r="B77" s="16" t="s">
+        <v>423</v>
+      </c>
+      <c r="C77" s="16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2813,7 +4482,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.48"/>
   </cols>
@@ -2875,7 +4544,7 @@
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.79"/>
@@ -3000,7 +4669,7 @@
       <c r="B2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3014,7 +4683,7 @@
       <c r="C3" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3028,7 +4697,7 @@
       <c r="C4" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3036,7 +4705,7 @@
       <c r="B5" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3046,7 +4715,7 @@
         <v>75</v>
       </c>
       <c r="C6" s="0"/>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3054,7 +4723,7 @@
       <c r="B7" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3068,7 +4737,7 @@
       <c r="C8" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3082,12 +4751,12 @@
       <c r="C9" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>83</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -3096,12 +4765,12 @@
       <c r="C10" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="4" t="s">
         <v>75</v>
       </c>
@@ -3123,7 +4792,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="4" t="s">
         <v>75</v>
       </c>
@@ -3135,7 +4804,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>84</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -3149,7 +4818,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>85</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -3175,7 +4844,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>87</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -3187,7 +4856,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -3199,7 +4868,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -3211,7 +4880,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6"/>
+      <c r="A20" s="5"/>
       <c r="B20" s="4" t="s">
         <v>75</v>
       </c>
@@ -3253,7 +4922,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="48.35"/>
   </cols>
@@ -3337,7 +5006,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
   </cols>
@@ -3392,7 +5061,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>83</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -3403,7 +5072,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="4" t="s">
         <v>75</v>
       </c>
@@ -3433,7 +5102,7 @@
       <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3444,7 +5113,7 @@
       <c r="A2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>95</v>
       </c>
     </row>
@@ -3491,11 +5160,11 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A51" activeCellId="0" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.22"/>
   </cols>
@@ -3542,7 +5211,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>102</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -3553,7 +5222,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>103</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -3586,7 +5255,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="4" t="s">
         <v>75</v>
       </c>
@@ -3595,7 +5264,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="4" t="s">
         <v>75</v>
       </c>
@@ -3615,7 +5284,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="4" t="s">
         <v>75</v>
       </c>
@@ -3624,7 +5293,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>107</v>
       </c>
       <c r="B12" s="0" t="s">
@@ -3635,7 +5304,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="4" t="s">
         <v>75</v>
       </c>
@@ -3644,7 +5313,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="4" t="s">
         <v>75</v>
       </c>
@@ -3664,7 +5333,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6"/>
+      <c r="A16" s="5"/>
       <c r="B16" s="4" t="s">
         <v>75</v>
       </c>
@@ -3695,7 +5364,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6"/>
+      <c r="A19" s="5"/>
       <c r="B19" s="4" t="s">
         <v>75</v>
       </c>
@@ -3704,7 +5373,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6"/>
+      <c r="A20" s="5"/>
       <c r="B20" s="4" t="s">
         <v>75</v>
       </c>
@@ -3713,7 +5382,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>111</v>
       </c>
       <c r="B21" s="0" t="s">
@@ -3724,7 +5393,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6"/>
+      <c r="A22" s="5"/>
       <c r="B22" s="4" t="s">
         <v>75</v>
       </c>
@@ -3733,7 +5402,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
         <v>112</v>
       </c>
       <c r="B23" s="0" t="s">
@@ -3755,7 +5424,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6"/>
+      <c r="A25" s="5"/>
       <c r="B25" s="4" t="s">
         <v>75</v>
       </c>
@@ -3764,7 +5433,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6"/>
+      <c r="A26" s="5"/>
       <c r="B26" s="4" t="s">
         <v>75</v>
       </c>
@@ -3773,7 +5442,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="9" t="s">
         <v>114</v>
       </c>
       <c r="B27" s="0" t="s">
@@ -3784,7 +5453,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6"/>
+      <c r="A28" s="5"/>
       <c r="B28" s="4" t="s">
         <v>75</v>
       </c>
@@ -3793,7 +5462,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="9" t="s">
         <v>115</v>
       </c>
       <c r="B29" s="0" t="s">
@@ -3815,7 +5484,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6"/>
+      <c r="A31" s="5"/>
       <c r="B31" s="4" t="s">
         <v>75</v>
       </c>
@@ -3824,7 +5493,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6"/>
+      <c r="A32" s="5"/>
       <c r="B32" s="4" t="s">
         <v>75</v>
       </c>
@@ -3833,7 +5502,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="9" t="s">
         <v>117</v>
       </c>
       <c r="B33" s="0" t="s">
@@ -3844,7 +5513,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6"/>
+      <c r="A34" s="5"/>
       <c r="B34" s="4" t="s">
         <v>75</v>
       </c>
@@ -3853,7 +5522,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="9" t="s">
         <v>118</v>
       </c>
       <c r="B35" s="0" t="s">
@@ -3875,7 +5544,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6"/>
+      <c r="A37" s="5"/>
       <c r="B37" s="4" t="s">
         <v>75</v>
       </c>
@@ -3889,6 +5558,170 @@
         <v>75</v>
       </c>
       <c r="D38" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5"/>
+      <c r="B40" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5"/>
+      <c r="B47" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5"/>
+      <c r="B50" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5"/>
+      <c r="B53" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D54" s="4" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added to map & content
</commit_message>
<xml_diff>
--- a/public/cges/content.xlsx
+++ b/public/cges/content.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Card Types" sheetId="1" state="hidden" r:id="rId2"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="447">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -179,6 +179,12 @@
     <t xml:space="preserve">/news</t>
   </si>
   <si>
+    <t xml:space="preserve">Women on Death Row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/wodr</t>
+  </si>
+  <si>
     <t xml:space="preserve">Defender Toolkit</t>
   </si>
   <si>
@@ -189,12 +195,6 @@
   </si>
   <si>
     <t xml:space="preserve">/resourcehub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Women on Death Row Worldwide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/wodr</t>
   </si>
   <si>
     <t xml:space="preserve">picture</t>
@@ -537,28 +537,46 @@
     <t xml:space="preserve">Manuals</t>
   </si>
   <si>
-    <t xml:space="preserve">FS Item</t>
+    <t xml:space="preserve">Melissa Lucio - Clemency Petition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melissa Lucio - Clemency Petition.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clemency Materials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lisa Montgomery - Petition to the Inter-American Commission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lisa Montgomery - Petition to the Inter-American Commission.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Litigation Tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primer On Transgender Individuals Facing the Death Penalty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capital punishment disproportionately targets socially marginalized individuals; it is no different for transgender people, who may face discrimination in every aspect of their lives. Accordingly, it is difficult to confirm how trans people who are on death row may have faced discrimination for being transgender in the criminal justice system. This factsheet provides an overview of the issues faced by transgender people who come into contact with the criminal justice system.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trans-Rights-and-Death-Penalty-Factsheet_V1.0-3.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Factsheets</t>
   </si>
   <si>
-    <t xml:space="preserve">Melissa Lucio - Clemency Petition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Melissa Lucio - Clemency Petition.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clemency Materials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lisa Montgomery - Petition to the Inter-American Commission</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lisa Montgomery - Petition to the Inter-American Commission.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Litigation Tools</t>
+    <t xml:space="preserve">Prison conditions for women facing the death penalty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a factsheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are at least 500 women on death row around the world, but they do not receive much attention in studies on the death penalty and the death row population. This factsheet examines the prison conditions that women on death row worldwide face, and includes profiles of women who were sentenced to death.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prison-conditions-for-women-facing-death-penalty.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">News Item</t>
@@ -618,25 +636,7 @@
     <t xml:space="preserve">Gender and Extreme Sentencing of Women </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Bibliography </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">8-14-24</t>
-    </r>
+    <t xml:space="preserve">Bibliography 8-14-24</t>
   </si>
   <si>
     <t xml:space="preserve">Bibliography - Gender and Extreme Sentencing of Women 8-14-2024.pdf</t>
@@ -669,6 +669,48 @@
     <t xml:space="preserve">Academic Articles</t>
   </si>
   <si>
+    <t xml:space="preserve">In the Extreme: Women Serving Life without Parole and Death Sentences in the United States</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The report is a joint publication of The Sentencing Project, National Black Women’s Justice Institute and the Cornell University Center on the Death Penalty Worldwide who together in 2020 formed the Alice Project. The collaboration seeks to highlight the experiences of incarcerated women and girls, to eliminate extreme sentences, and to reduce the influence of racial and gender bias in the criminal legal system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In-the-Extreme-Women-Serving-Life-without-Parole-and-Death-Sentences-in-the-United-States-1.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mass Release Now: New York State’s Obligation to Deliver Reparations for Criminalized Survivors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For this report, Survived &amp; Punished NY (S&amp;P NY) and the International Human Rights Clinic at Cornell Law School surveyed and interviewed members of S&amp;P NY who are incarcerated in NYS and identify as survivors of GBV. The report examines how these survivors struggled to escape GBV because they did not receive even the most basic resources or support to create safety for themselves. Without this infrastructure, they resorted to conduct that has been criminalized. The report analyzes how New York State, by criminalizing survivors for conduct that occurred under circumstances the state could have prevented, perpetuates gender-based discrimination and gender-based violence.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mass-Release-Now-Report-Final-2021.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Judged for More Than Her Crime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Global Overview of Women Facing the Death Penalty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cases of women condemned to death have revealed significant patterns of arbitrariness and gender-based discrimination in the application of the death penalty to women worldwide. This report illuminates these patterns and how gender creates uniquely precarious conditions for women facing capital sentences.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Judged-More-Than-Her-Crime.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Justice Denied</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Global Study of Wrongful Death Row Convictions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This report explores the phenomenon of wrongful convictions in six different jurisdictions representing a range of geographic regions, judicial traditions, and political contexts. It identifies the systemic factors in each country that increase the likelihood that innocent persons will be sentenced to death.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Justice-Denied-A-Global-Study-of-Wrongful-Death-Row-Convictions.pdf</t>
+  </si>
+  <si>
     <t xml:space="preserve">Women on Death Row: </t>
   </si>
   <si>
@@ -885,6 +927,9 @@
     <t xml:space="preserve">Crime</t>
   </si>
   <si>
+    <t xml:space="preserve">Legend</t>
+  </si>
+  <si>
     <t xml:space="preserve">Afghanistan</t>
   </si>
   <si>
@@ -894,10 +939,16 @@
     <t xml:space="preserve">Murder</t>
   </si>
   <si>
+    <t xml:space="preserve">Retentionist</t>
+  </si>
+  <si>
     <t xml:space="preserve">Algeria</t>
   </si>
   <si>
     <t xml:space="preserve">DZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De facto abolitionist</t>
   </si>
   <si>
     <t xml:space="preserve">Antigua and Barbuda</t>
@@ -1483,23 +1534,17 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1513,6 +1558,14 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1559,7 +1612,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1604,28 +1657,32 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1655,7 +1712,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1825,7 +1882,7 @@
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -1915,7 +1972,7 @@
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1988,7 +2045,7 @@
       <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.27"/>
@@ -2078,11 +2135,11 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
   </cols>
@@ -2137,15 +2194,15 @@
         <v>141</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
@@ -2155,37 +2212,44 @@
         <v>141</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
-        <v>140</v>
-      </c>
+      <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="A6" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>158</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2209,7 +2273,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2232,7 +2296,7 @@
       <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2262,7 +2326,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>139</v>
@@ -2314,9 +2378,9 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2344,7 +2408,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>53</v>
@@ -2358,7 +2422,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>80</v>
@@ -2368,8 +2432,8 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
-        <v>160</v>
+      <c r="A5" s="13" t="s">
+        <v>166</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>53</v>
@@ -2379,13 +2443,13 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="128.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>161</v>
+      <c r="A6" s="14" t="s">
+        <v>167</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="4" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2400,7 +2464,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>80</v>
@@ -2443,13 +2507,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="65.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="63.21"/>
@@ -2478,10 +2542,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>140</v>
@@ -2490,18 +2554,18 @@
         <v>141</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>166</v>
+        <v>171</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>168</v>
+        <v>173</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>174</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>140</v>
@@ -2510,18 +2574,18 @@
         <v>141</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>170</v>
+        <v>175</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>172</v>
+        <v>177</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>140</v>
@@ -2529,11 +2593,73 @@
       <c r="D4" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>174</v>
+      <c r="E4" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2558,7 +2684,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.18"/>
   </cols>
@@ -2595,7 +2721,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>53</v>
@@ -2610,7 +2736,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>80</v>
@@ -2800,7 +2926,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.18"/>
   </cols>
@@ -2833,7 +2959,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>139</v>
@@ -2856,10 +2982,10 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>36</v>
@@ -2867,10 +2993,10 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>36</v>
@@ -2878,10 +3004,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>36</v>
@@ -2889,10 +3015,10 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>36</v>
@@ -2900,10 +3026,10 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>36</v>
@@ -2911,10 +3037,10 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>36</v>
@@ -2922,10 +3048,10 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>36</v>
@@ -2933,10 +3059,10 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>36</v>
@@ -2944,10 +3070,10 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>36</v>
@@ -2955,10 +3081,10 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>36</v>
@@ -2966,10 +3092,10 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>36</v>
@@ -2977,10 +3103,10 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>36</v>
@@ -2988,10 +3114,10 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>36</v>
@@ -2999,10 +3125,10 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>36</v>
@@ -3010,10 +3136,10 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>36</v>
@@ -3021,10 +3147,10 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>36</v>
@@ -3032,10 +3158,10 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>36</v>
@@ -3043,10 +3169,10 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>36</v>
@@ -3054,10 +3180,10 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>36</v>
@@ -3065,10 +3191,10 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>36</v>
@@ -3076,10 +3202,10 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>36</v>
@@ -3087,10 +3213,10 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>36</v>
@@ -3098,10 +3224,10 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>36</v>
@@ -3109,10 +3235,10 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>36</v>
@@ -3120,10 +3246,10 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>36</v>
@@ -3131,10 +3257,10 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>36</v>
@@ -3142,10 +3268,10 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>36</v>
@@ -3153,10 +3279,10 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>36</v>
@@ -3164,10 +3290,10 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="B31" s="0" t="s">
         <v>209</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>189</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>36</v>
@@ -3175,10 +3301,10 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>36</v>
@@ -3186,10 +3312,10 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>36</v>
@@ -3197,10 +3323,10 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>36</v>
@@ -3208,10 +3334,10 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>36</v>
@@ -3219,10 +3345,10 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>36</v>
@@ -3230,10 +3356,10 @@
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>36</v>
@@ -3241,10 +3367,10 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>36</v>
@@ -3252,10 +3378,10 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>36</v>
@@ -3263,10 +3389,10 @@
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>223</v>
+        <v>243</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>36</v>
@@ -3274,10 +3400,10 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>36</v>
@@ -3285,10 +3411,10 @@
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>36</v>
@@ -3296,10 +3422,10 @@
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>229</v>
+        <v>249</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>36</v>
@@ -3307,10 +3433,10 @@
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>36</v>
@@ -3318,10 +3444,10 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>232</v>
+        <v>252</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>233</v>
+        <v>253</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>36</v>
@@ -3329,10 +3455,10 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>234</v>
+        <v>254</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>36</v>
@@ -3340,10 +3466,10 @@
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>36</v>
@@ -3351,10 +3477,10 @@
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>36</v>
@@ -3362,10 +3488,10 @@
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>36</v>
@@ -3373,10 +3499,10 @@
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>36</v>
@@ -3384,10 +3510,10 @@
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>36</v>
@@ -3395,10 +3521,10 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="H52" s="0" t="s">
         <v>36</v>
@@ -3423,10 +3549,10 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.82"/>
@@ -3467,6 +3593,12 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="F5" s="1"/>
     </row>
   </sheetData>
@@ -3485,10 +3617,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C48" activeCellId="0" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3501,963 +3633,1194 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>246</v>
+        <v>266</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>247</v>
+        <v>268</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>248</v>
+        <v>269</v>
       </c>
       <c r="C2" s="16" t="n">
         <v>5</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>249</v>
+        <v>270</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>250</v>
+        <v>272</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="C3" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E3" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>252</v>
+        <v>275</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
       <c r="C4" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E4" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
       <c r="C5" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E5" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
-        <v>256</v>
+        <v>279</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>257</v>
+        <v>280</v>
       </c>
       <c r="C6" s="16" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>249</v>
+        <v>270</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
-        <v>258</v>
+        <v>281</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>259</v>
+        <v>282</v>
       </c>
       <c r="C7" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E7" s="0" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
-        <v>260</v>
+        <v>283</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>261</v>
+        <v>284</v>
       </c>
       <c r="C8" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E8" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="16" t="s">
-        <v>262</v>
+        <v>285</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>263</v>
+        <v>286</v>
       </c>
       <c r="C9" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E9" s="0" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="16" t="s">
-        <v>264</v>
+        <v>287</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>265</v>
+        <v>288</v>
       </c>
       <c r="C10" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E10" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="16" t="s">
-        <v>266</v>
+        <v>289</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>267</v>
+        <v>290</v>
       </c>
       <c r="C11" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E11" s="0" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="16" t="s">
-        <v>268</v>
+        <v>291</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>269</v>
+        <v>292</v>
       </c>
       <c r="C12" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E12" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="16" t="s">
-        <v>270</v>
+        <v>293</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>271</v>
+        <v>294</v>
       </c>
       <c r="C13" s="16" t="n">
         <v>14</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>272</v>
+        <v>295</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="16" t="s">
-        <v>273</v>
+        <v>296</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>274</v>
+        <v>297</v>
       </c>
       <c r="C14" s="16" t="n">
         <v>56</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>275</v>
+        <v>298</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="16" t="s">
-        <v>276</v>
+        <v>299</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>277</v>
+        <v>300</v>
       </c>
       <c r="C15" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E15" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="16" t="s">
-        <v>278</v>
+        <v>301</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>279</v>
+        <v>302</v>
       </c>
       <c r="C16" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E16" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="16" t="s">
-        <v>280</v>
+        <v>303</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>281</v>
+        <v>304</v>
       </c>
       <c r="C17" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E17" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="16" t="s">
-        <v>282</v>
+        <v>305</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>283</v>
+        <v>306</v>
       </c>
       <c r="C18" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E18" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="s">
-        <v>284</v>
+        <v>307</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>285</v>
+        <v>308</v>
       </c>
       <c r="C19" s="16" t="n">
         <v>146</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>286</v>
+        <v>309</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
-        <v>287</v>
+        <v>310</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>288</v>
+        <v>311</v>
       </c>
       <c r="C20" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E20" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
-        <v>289</v>
+        <v>312</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
       <c r="C21" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E21" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
-        <v>291</v>
+        <v>314</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>292</v>
+        <v>315</v>
       </c>
       <c r="C22" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E22" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
-        <v>293</v>
+        <v>316</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>294</v>
+        <v>317</v>
       </c>
       <c r="C23" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E23" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="16" t="s">
-        <v>295</v>
+        <v>318</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>296</v>
+        <v>319</v>
       </c>
       <c r="C24" s="16" t="n">
         <v>2</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>275</v>
+        <v>298</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="16" t="s">
-        <v>297</v>
+        <v>320</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>298</v>
+        <v>321</v>
       </c>
       <c r="C25" s="16" t="n">
         <v>12</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>275</v>
+        <v>298</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="16" t="s">
-        <v>299</v>
+        <v>322</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>300</v>
+        <v>323</v>
       </c>
       <c r="C26" s="16" t="n">
         <v>7</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>301</v>
+        <v>324</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="16" t="s">
-        <v>302</v>
+        <v>325</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>303</v>
+        <v>326</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>275</v>
+        <v>298</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="16" t="s">
-        <v>305</v>
+        <v>328</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>306</v>
+        <v>329</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>307</v>
+        <v>330</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>308</v>
+        <v>331</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="16" t="s">
-        <v>309</v>
+        <v>332</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>310</v>
+        <v>333</v>
       </c>
       <c r="C29" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E29" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="16" t="s">
-        <v>311</v>
+        <v>334</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>312</v>
+        <v>335</v>
       </c>
       <c r="C30" s="16" t="n">
         <v>7</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>313</v>
+        <v>336</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="16" t="s">
-        <v>314</v>
+        <v>337</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>315</v>
+        <v>338</v>
       </c>
       <c r="C31" s="16" t="n">
         <v>20</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>308</v>
+        <v>331</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="16" t="s">
-        <v>316</v>
+        <v>339</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>317</v>
+        <v>340</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>318</v>
+        <v>341</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>249</v>
+        <v>270</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="16" t="s">
-        <v>319</v>
+        <v>342</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>320</v>
+        <v>343</v>
       </c>
       <c r="C33" s="16" t="n">
         <v>6</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>249</v>
+        <v>270</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="16" t="s">
-        <v>321</v>
+        <v>344</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>322</v>
+        <v>345</v>
       </c>
       <c r="C34" s="16" t="n">
         <v>1</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>323</v>
+        <v>346</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="16" t="s">
-        <v>324</v>
+        <v>347</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>325</v>
+        <v>348</v>
       </c>
       <c r="C35" s="16" t="n">
         <v>1</v>
       </c>
+      <c r="E35" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="16" t="s">
-        <v>326</v>
+        <v>349</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>327</v>
+        <v>350</v>
       </c>
       <c r="C36" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E36" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="16" t="s">
-        <v>328</v>
+        <v>351</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>329</v>
+        <v>352</v>
       </c>
       <c r="C37" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E37" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="16" t="s">
-        <v>330</v>
+        <v>353</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>331</v>
+        <v>354</v>
       </c>
       <c r="C38" s="16" t="n">
         <v>3</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>249</v>
+        <v>270</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="16" t="s">
-        <v>332</v>
+        <v>355</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>333</v>
+        <v>356</v>
       </c>
       <c r="C39" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E39" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="16" t="s">
-        <v>334</v>
+        <v>357</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>335</v>
+        <v>358</v>
       </c>
       <c r="C40" s="16" t="n">
         <v>143</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>301</v>
+        <v>324</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="16" t="s">
-        <v>336</v>
+        <v>359</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>337</v>
+        <v>360</v>
       </c>
       <c r="C41" s="16" t="n">
         <v>1</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>338</v>
+        <v>361</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="16" t="s">
-        <v>339</v>
+        <v>362</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>340</v>
+        <v>363</v>
       </c>
       <c r="C42" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E42" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="16" t="s">
-        <v>341</v>
+        <v>364</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>342</v>
+        <v>365</v>
       </c>
       <c r="C43" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E43" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="16" t="s">
-        <v>343</v>
+        <v>366</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>344</v>
+        <v>367</v>
       </c>
       <c r="C44" s="16" t="n">
         <v>10</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>249</v>
+        <v>270</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="16" t="s">
-        <v>345</v>
+        <v>368</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>346</v>
+        <v>369</v>
       </c>
       <c r="C45" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E45" s="0" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="16" t="s">
-        <v>347</v>
+        <v>370</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>348</v>
+        <v>371</v>
       </c>
       <c r="C46" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E46" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="16" t="s">
-        <v>349</v>
+        <v>372</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>350</v>
+        <v>373</v>
       </c>
       <c r="C47" s="16" t="n">
         <v>32</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>249</v>
+        <v>270</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="16" t="s">
-        <v>351</v>
+        <v>374</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>352</v>
+        <v>375</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>353</v>
+        <v>376</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>275</v>
+        <v>298</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="16" t="s">
-        <v>354</v>
+        <v>377</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>355</v>
+        <v>378</v>
       </c>
       <c r="C49" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E49" s="0" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="16" t="s">
-        <v>356</v>
+        <v>379</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>357</v>
+        <v>380</v>
       </c>
       <c r="C50" s="16" t="n">
         <v>29</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>249</v>
+        <v>270</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="16" t="s">
-        <v>358</v>
+        <v>381</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>359</v>
+        <v>382</v>
       </c>
       <c r="C51" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E51" s="0" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="16" t="s">
-        <v>360</v>
+        <v>383</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>361</v>
+        <v>384</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>362</v>
+        <v>385</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>275</v>
+        <v>298</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="16" t="s">
-        <v>363</v>
+        <v>386</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>364</v>
+        <v>387</v>
       </c>
       <c r="C53" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E53" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="16" t="s">
-        <v>365</v>
+        <v>388</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>366</v>
+        <v>389</v>
       </c>
       <c r="C54" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E54" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="16" t="s">
-        <v>367</v>
+        <v>390</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>368</v>
+        <v>391</v>
       </c>
       <c r="C55" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E55" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="16" t="s">
-        <v>369</v>
+        <v>392</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>370</v>
+        <v>393</v>
       </c>
       <c r="C56" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E56" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="16" t="s">
-        <v>371</v>
+        <v>394</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>372</v>
+        <v>395</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>373</v>
+        <v>396</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="16" t="s">
-        <v>374</v>
+        <v>397</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>375</v>
+        <v>398</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>376</v>
+        <v>399</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>377</v>
+        <v>400</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="16" t="s">
-        <v>378</v>
+        <v>401</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>379</v>
+        <v>402</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>353</v>
+        <v>376</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="16" t="s">
-        <v>380</v>
+        <v>403</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>381</v>
+        <v>404</v>
       </c>
       <c r="C60" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E60" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="16" t="s">
-        <v>382</v>
+        <v>405</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>383</v>
+        <v>406</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>384</v>
+        <v>407</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>275</v>
+        <v>298</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="16" t="s">
-        <v>385</v>
+        <v>408</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>386</v>
+        <v>409</v>
       </c>
       <c r="C62" s="16" t="n">
         <v>84</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>275</v>
+        <v>298</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="16" t="s">
-        <v>387</v>
+        <v>410</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>388</v>
+        <v>411</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>389</v>
+        <v>412</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>390</v>
+        <v>413</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="16" t="s">
-        <v>391</v>
+        <v>414</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>392</v>
+        <v>415</v>
       </c>
       <c r="C64" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E64" s="0" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="16" t="s">
-        <v>393</v>
+        <v>416</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>394</v>
+        <v>417</v>
       </c>
       <c r="C65" s="16" t="n">
         <v>1</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>249</v>
+        <v>270</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="16" t="s">
-        <v>395</v>
+        <v>418</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>396</v>
+        <v>419</v>
       </c>
       <c r="C66" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E66" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="16" t="s">
-        <v>397</v>
+        <v>420</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>398</v>
+        <v>421</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>399</v>
+        <v>422</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>249</v>
+        <v>270</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="16" t="s">
-        <v>400</v>
+        <v>423</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>401</v>
+        <v>424</v>
       </c>
       <c r="C68" s="16" t="n">
         <v>33</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>301</v>
+        <v>324</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="16" t="s">
-        <v>402</v>
+        <v>425</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>403</v>
+        <v>426</v>
       </c>
       <c r="C69" s="16" t="n">
         <v>0</v>
       </c>
+      <c r="E69" s="0" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="16" t="s">
-        <v>404</v>
+        <v>427</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>405</v>
+        <v>428</v>
       </c>
       <c r="C70" s="16" t="n">
         <v>1</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>249</v>
+        <v>270</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="16" t="s">
-        <v>406</v>
+        <v>429</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>407</v>
+        <v>430</v>
       </c>
       <c r="C71" s="16" t="s">
-        <v>275</v>
+        <v>298</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="16" t="s">
-        <v>408</v>
+        <v>431</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>409</v>
+        <v>432</v>
       </c>
       <c r="C72" s="16" t="n">
         <v>4</v>
       </c>
       <c r="D72" s="16" t="s">
-        <v>249</v>
+        <v>270</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="16" t="s">
-        <v>410</v>
+        <v>433</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>411</v>
+        <v>434</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>412</v>
+        <v>435</v>
       </c>
       <c r="D73" s="16" t="s">
-        <v>377</v>
+        <v>400</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="16" t="s">
-        <v>413</v>
+        <v>436</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>414</v>
+        <v>437</v>
       </c>
       <c r="C74" s="16" t="n">
         <v>52</v>
       </c>
       <c r="D74" s="16" t="s">
-        <v>249</v>
+        <v>270</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="16" t="s">
-        <v>415</v>
+        <v>438</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>416</v>
+        <v>439</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>417</v>
+        <v>440</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>418</v>
+        <v>441</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="16" t="s">
-        <v>419</v>
+        <v>442</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>420</v>
+        <v>443</v>
       </c>
       <c r="C76" s="16" t="n">
         <v>2</v>
       </c>
       <c r="D76" s="16" t="s">
-        <v>421</v>
+        <v>444</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="16" t="s">
-        <v>422</v>
+        <v>445</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>423</v>
+        <v>446</v>
       </c>
       <c r="C77" s="16" t="n">
         <v>0</v>
+      </c>
+      <c r="E77" s="0" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -4479,10 +4842,10 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.48"/>
   </cols>
@@ -4497,25 +4860,17 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="2" t="s">
         <v>51</v>
       </c>
     </row>
@@ -4544,7 +4899,7 @@
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.79"/>
@@ -4922,7 +5277,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="48.35"/>
   </cols>
@@ -5006,7 +5361,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.02"/>
   </cols>
@@ -5102,7 +5457,7 @@
       <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5160,11 +5515,11 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A51" activeCellId="0" sqref="A51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A53" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A54" activeCellId="0" sqref="A54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.22"/>
   </cols>

</xml_diff>